<commit_message>
Updated as per new guidelines
</commit_message>
<xml_diff>
--- a/documents/Published/Rotating Chart/RotatingChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Rotating Chart/RotatingChartByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\Rotating Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\Rotating Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E99D9-88D6-4AC9-92DA-412A9E59A37F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035FC417-C7B5-4DEA-8B81-4B0DA774DAFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" xr2:uid="{67278F39-5C2F-4C21-84D9-7B8CB41EFB1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67278F39-5C2F-4C21-84D9-7B8CB41EFB1B}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>S no</t>
   </si>
@@ -272,6 +272,20 @@
 2. Go to 'Animation Setting' option
 3. Set toggle to ON.
 4. Update 'Delay' to 4</t>
+  </si>
+  <si>
+    <t>Drillthrough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Generate a chart with some data
+2.Create new report page and in DrillThrough add the fields for drillthrough.
+3. Right click on the chart, select the Drillthrough option from the menu. </t>
+  </si>
+  <si>
+    <t>Created custom menu to drillthrough from one visual to another.</t>
+  </si>
+  <si>
+    <t>1. On right click of the chart and selecting the Drillthrough option from the context-menu , the report will drillthrough to the newly created report page.</t>
   </si>
 </sst>
 </file>
@@ -403,13 +417,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -438,9 +451,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -776,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DFE4D4-682B-4136-8526-C2C15BB103EA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,19 +818,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -890,6 +900,23 @@
       </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -912,284 +939,284 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="18"/>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="14">
         <v>18</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="18"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>19</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="12">
         <v>20</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="13">
         <v>21</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="13" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>